<commit_message>
continue writing to full grav excel
</commit_message>
<xml_diff>
--- a/pendulum/full_obs_pendulum/full_obs_grav.xlsx
+++ b/pendulum/full_obs_pendulum/full_obs_grav.xlsx
@@ -3,11 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="500" windowWidth="18200" windowHeight="8500" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="500" windowWidth="18200" windowHeight="8500" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="9.81" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="11" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="12" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -5241,4 +5243,1032 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>conditional(add(y, y), add(conditional(x, conditional(conditional(y, x), add(vel, vel))), add(add(x, add(vel, add(conditional(conditional(conditional(x, vel), conditional(vel, vel)), conditional(x, x)), add(x, x)))), add(y, y))))</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>-1244.91</v>
+      </c>
+      <c r="C1" t="n">
+        <v>-1182.54</v>
+      </c>
+      <c r="D1" t="n">
+        <v>-935.77</v>
+      </c>
+      <c r="E1" t="n">
+        <v>-1437.9</v>
+      </c>
+      <c r="F1" t="n">
+        <v>-1662.46</v>
+      </c>
+      <c r="G1" t="n">
+        <v>-1600.89</v>
+      </c>
+      <c r="H1" t="n">
+        <v>-1502.35</v>
+      </c>
+      <c r="I1" t="n">
+        <v>-1631.74</v>
+      </c>
+      <c r="J1" t="n">
+        <v>-1815.57</v>
+      </c>
+      <c r="K1" t="n">
+        <v>-1902.44</v>
+      </c>
+      <c r="L1" t="n">
+        <v>-1968.06</v>
+      </c>
+      <c r="M1" t="n">
+        <v>-2022.6</v>
+      </c>
+      <c r="N1" t="n">
+        <v>-2044.17</v>
+      </c>
+      <c r="O1" t="n">
+        <v>-2143.11</v>
+      </c>
+      <c r="P1" t="n">
+        <v>-2195.58</v>
+      </c>
+      <c r="Q1" t="n">
+        <v>-2211.44</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>conditional(add(y, y), add(add(add(add(x, y), x), add(add(x, add(x, x)), y)), vel))</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-1107.55</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-1216.59</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-1267.9</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-1468.39</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-1689.83</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-1664.02</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-1594.55</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-1514.33</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-1803.23</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-1920.47</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-1941.31</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-2002.31</v>
+      </c>
+      <c r="N2" t="n">
+        <v>-2066.33</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-2166.54</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-2174.14</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-2212.99</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>add(conditional(add(y, y), add(add(add(conditional(conditional(x, y), conditional(vel, conditional(x, add(x, vel)))), add(add(x, add(vel, x)), vel)), add(x, y)), add(add(x, x), x))), conditional(conditional(y, y), add(add(add(add(conditional(x, conditional(conditional(y, conditional(add(x, y), add(y, y))), vel)), add(x, vel)), add(x, conditional(conditional(x, add(y, y)), conditional(conditional(conditional(vel, x), vel), add(y, x))))), add(add(x, x), conditional(add(conditional(x, x), y), add(x, conditional(y, y))))), y)))</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>-1264.06</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-1177.72</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-1114.32</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-1204.95</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-1357.91</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-1446.38</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-1317.76</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-1331.27</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-1772.33</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-1930.66</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-1929</v>
+      </c>
+      <c r="M3" t="n">
+        <v>-1998.95</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-2029.1</v>
+      </c>
+      <c r="O3" t="n">
+        <v>-2118.43</v>
+      </c>
+      <c r="P3" t="n">
+        <v>-2175.85</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-2207.69</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>conditional(add(y, y), add(conditional(conditional(conditional(conditional(x, vel), conditional(add(vel, x), conditional(y, x))), conditional(conditional(add(conditional(x, x), vel), x), vel)), y), add(add(x, y), add(add(vel, add(x, add(y, x))), conditional(x, x)))))</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-1210.09</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-1105.84</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-1260.36</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-1531.08</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-1954.74</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-2056.67</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-1899.43</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-1895.74</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-1914.2</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-1939.47</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-2033.78</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-2032.25</v>
+      </c>
+      <c r="N4" t="n">
+        <v>-2092.22</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-2143.18</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-2179.92</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-2239.04</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>add(conditional(y, add(x, vel)), conditional(add(y, y), add(add(add(add(x, add(conditional(add(y, x), add(y, x)), x)), x), add(vel, conditional(y, y))), conditional(add(conditional(x, conditional(vel, add(y, conditional(add(vel, y), x)))), x), conditional(vel, add(add(vel, x), conditional(add(y, y), conditional(add(conditional(y, vel), conditional(x, vel)), add(x, vel)))))))))</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-1129.42</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-1444.57</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-1495.71</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-1581.78</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-1615.55</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-1836.78</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-1768.99</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-1773.55</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-1525.25</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-1854.48</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-1951.71</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-2010.4</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-2041.71</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-2101.52</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-2180.93</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-2216.04</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>conditional(add(y, add(y, y)), add(add(add(y, add(conditional(conditional(x, x), add(add(add(add(add(add(x, y), add(conditional(vel, y), add(x, add(add(vel, add(vel, x)), conditional(y, y))))), conditional(y, x)), add(x, x)), add(add(y, conditional(x, conditional(add(y, vel), conditional(y, y)))), conditional(x, x))), conditional(conditional(add(vel, x), conditional(x, x)), add(y, y)))), add(x, y))), add(x, x)), add(x, add(add(vel, x), conditional(conditional(y, x), y)))))</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-1207.71</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-1188.63</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-1215.32</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-1169.53</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-1414.98</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-1520.92</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-1502.04</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-1596.81</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-1809.02</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-1919.52</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-1978.17</v>
+      </c>
+      <c r="M6" t="n">
+        <v>-2033.31</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-2081.88</v>
+      </c>
+      <c r="O6" t="n">
+        <v>-2159.23</v>
+      </c>
+      <c r="P6" t="n">
+        <v>-2167.15</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-2233.17</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>conditional(add(conditional(y, y), add(y, y)), add(add(add(add(add(x, x), add(vel, x)), add(add(conditional(x, vel), x), add(x, add(add(add(add(add(vel, x), add(x, y)), add(add(x, vel), add(vel, conditional(vel, vel)))), add(add(add(add(add(add(add(x, x), add(y, y)), add(x, add(vel, add(add(y, vel), add(x, x))))), add(add(x, x), add(x, x))), x), x), x)), add(x, x))))), add(add(x, x), x)), x))</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>-1216.19</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-1202.22</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-1449.54</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-1371.71</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-1600.73</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-1748.33</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-1347.65</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-1623.82</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-1790.96</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-1886.58</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-1928.33</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-2006.09</v>
+      </c>
+      <c r="N7" t="n">
+        <v>-2095.52</v>
+      </c>
+      <c r="O7" t="n">
+        <v>-2128.8</v>
+      </c>
+      <c r="P7" t="n">
+        <v>-2167.31</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-2185.62</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>conditional(add(conditional(x, add(x, conditional(conditional(x, x), add(conditional(conditional(y, add(y, vel)), conditional(add(add(x, add(conditional(conditional(x, conditional(x, add(vel, x))), add(add(conditional(add(vel, x), conditional(vel, y)), x), add(y, vel))), y)), y), y)), add(x, add(y, y)))))), add(y, y)), add(add(add(add(x, y), y), x), add(vel, x)))</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-1190.17</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-1110.45</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-1096.64</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-1139.21</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-1307.03</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-1337.22</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-1221.97</v>
+      </c>
+      <c r="I8" t="n">
+        <v>-1033.82</v>
+      </c>
+      <c r="J8" t="n">
+        <v>-1638.99</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-1764.54</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-1829.76</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-1883.99</v>
+      </c>
+      <c r="N8" t="n">
+        <v>-1982.36</v>
+      </c>
+      <c r="O8" t="n">
+        <v>-2024.19</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-2086.97</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-2167.99</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>conditional(add(y, y), add(add(x, y), add(add(conditional(conditional(conditional(x, add(y, add(vel, x))), add(add(x, x), x)), add(x, add(y, y))), add(conditional(y, y), vel)), add(conditional(x, x), conditional(x, x)))))</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-1371.04</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-1240.46</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-1039.53</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-1269.1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-1312.16</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-1241.11</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-1528.74</v>
+      </c>
+      <c r="I9" t="n">
+        <v>-1529.18</v>
+      </c>
+      <c r="J9" t="n">
+        <v>-1731.15</v>
+      </c>
+      <c r="K9" t="n">
+        <v>-1914.64</v>
+      </c>
+      <c r="L9" t="n">
+        <v>-1938.13</v>
+      </c>
+      <c r="M9" t="n">
+        <v>-1977.21</v>
+      </c>
+      <c r="N9" t="n">
+        <v>-2048.92</v>
+      </c>
+      <c r="O9" t="n">
+        <v>-2104.07</v>
+      </c>
+      <c r="P9" t="n">
+        <v>-2181.33</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>-2198.5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>conditional(add(add(y, y), y), add(add(add(x, vel), add(add(add(add(add(x, add(vel, add(x, add(x, x)))), add(add(y, add(y, vel)), add(x, add(add(conditional(x, x), conditional(y, y)), conditional(add(vel, x), conditional(vel, conditional(add(y, vel), add(y, vel)))))))), add(add(x, add(x, conditional(x, vel))), conditional(x, conditional(x, add(x, add(x, x)))))), add(x, x)), add(x, add(add(conditional(x, x), conditional(y, vel)), conditional(conditional(vel, vel), vel))))), add(add(x, add(x, x)), conditional(x, add(y, y)))))</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-1305.89</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-1331.15</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-1380.47</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-1367.48</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-1657.79</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-1953.13</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-2075.77</v>
+      </c>
+      <c r="I10" t="n">
+        <v>-2156.55</v>
+      </c>
+      <c r="J10" t="n">
+        <v>-2034.84</v>
+      </c>
+      <c r="K10" t="n">
+        <v>-1982.33</v>
+      </c>
+      <c r="L10" t="n">
+        <v>-2060.46</v>
+      </c>
+      <c r="M10" t="n">
+        <v>-2128.71</v>
+      </c>
+      <c r="N10" t="n">
+        <v>-2079.07</v>
+      </c>
+      <c r="O10" t="n">
+        <v>-2135</v>
+      </c>
+      <c r="P10" t="n">
+        <v>-2221.96</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>-2239.86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>conditional(add(y, y), add(add(add(y, x), conditional(conditional(y, y), y)), add(vel, add(add(add(add(x, x), conditional(conditional(x, x), conditional(x, vel))), conditional(x, add(add(conditional(conditional(vel, y), add(x, conditional(x, x))), add(add(add(conditional(add(x, vel), add(conditional(y, y), vel)), x), add(x, y)), add(vel, add(x, x)))), add(add(x, conditional(add(y, add(add(y, add(x, x)), y)), add(vel, vel))), conditional(x, x))))), x))))</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>-1153.42</v>
+      </c>
+      <c r="C1" t="n">
+        <v>-1114.02</v>
+      </c>
+      <c r="D1" t="n">
+        <v>-1031.71</v>
+      </c>
+      <c r="E1" t="n">
+        <v>-1182.4</v>
+      </c>
+      <c r="F1" t="n">
+        <v>-1292.69</v>
+      </c>
+      <c r="G1" t="n">
+        <v>-1227.98</v>
+      </c>
+      <c r="H1" t="n">
+        <v>-1482.45</v>
+      </c>
+      <c r="I1" t="n">
+        <v>-1662.67</v>
+      </c>
+      <c r="J1" t="n">
+        <v>-1830.02</v>
+      </c>
+      <c r="K1" t="n">
+        <v>-1909.82</v>
+      </c>
+      <c r="L1" t="n">
+        <v>-1901.46</v>
+      </c>
+      <c r="M1" t="n">
+        <v>-1980.47</v>
+      </c>
+      <c r="N1" t="n">
+        <v>-2003.76</v>
+      </c>
+      <c r="O1" t="n">
+        <v>-2092.23</v>
+      </c>
+      <c r="P1" t="n">
+        <v>-2175.86</v>
+      </c>
+      <c r="Q1" t="n">
+        <v>-2190.39</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>conditional(add(conditional(x, add(conditional(add(y, conditional(conditional(vel, vel), add(vel, x))), add(add(add(x, vel), add(x, add(x, vel))), y)), add(add(y, x), conditional(x, vel)))), add(y, y)), add(add(x, vel), add(y, add(x, y))))</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-1785.29</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-1925.46</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-2300.69</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-2544.62</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-2544.66</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-2510.69</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-2437.01</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-2344.5</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-2246.4</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-2141.51</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-2028.35</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-1587.12</v>
+      </c>
+      <c r="N2" t="n">
+        <v>-1771.25</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-1807.53</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-1769.38</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-2025.53</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>conditional(add(add(y, y), conditional(y, y)), add(add(add(conditional(x, vel), y), add(add(vel, x), add(conditional(y, y), conditional(x, x)))), add(add(y, x), add(conditional(x, x), conditional(x, x)))))</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>-1265.81</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-1212.77</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-1329.2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-1269.77</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-1359.98</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-1512.32</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-1464.49</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-1516.71</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-1775.76</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-1927.53</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-1969.96</v>
+      </c>
+      <c r="M3" t="n">
+        <v>-2012.38</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-2058.7</v>
+      </c>
+      <c r="O3" t="n">
+        <v>-2094.39</v>
+      </c>
+      <c r="P3" t="n">
+        <v>-2188.33</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-2194.04</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>add(conditional(conditional(x, vel), add(x, x)), conditional(add(y, y), add(add(vel, add(conditional(conditional(x, y), conditional(conditional(conditional(x, add(conditional(vel, add(add(vel, vel), conditional(x, y))), add(vel, conditional(x, conditional(conditional(x, vel), add(x, x)))))), add(vel, x)), conditional(y, add(conditional(y, x), conditional(add(vel, conditional(x, y)), x))))), add(add(x, y), add(x, add(x, x))))), y)))</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-2304.58</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-2348.73</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-2331.56</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-2330.86</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-2368.74</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-2266.57</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-2233.8</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-1954.23</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-1878.25</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-2144.08</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-2053.36</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-1662.16</v>
+      </c>
+      <c r="N4" t="n">
+        <v>-1755.38</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-1833.93</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-1849.48</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-2033.63</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>add(conditional(x, add(vel, add(add(y, x), conditional(conditional(vel, x), add(x, y))))), conditional(add(y, add(y, y)), add(add(add(add(add(x, conditional(conditional(x, add(conditional(x, x), conditional(conditional(x, vel), add(conditional(x, y), add(x, x))))), add(conditional(y, vel), vel))), add(add(x, x), add(x, y))), add(x, conditional(add(x, y), conditional(x, x)))), add(x, add(add(conditional(x, x), add(vel, add(x, y))), vel))), x)))</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-1086.21</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-1016.12</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-821.5700000000001</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-968.16</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-1222.27</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-1271.72</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-1160.51</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-1040.63</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-596.37</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-1131.75</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-1381.04</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-1574.01</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-1741.91</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-1808.34</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-1992.16</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-2056.4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>add(conditional(x, conditional(vel, conditional(conditional(conditional(add(x, vel), conditional(conditional(add(vel, x), add(x, conditional(conditional(x, y), conditional(y, y)))), vel)), conditional(add(x, conditional(add(x, vel), add(vel, vel))), y)), add(conditional(y, y), add(y, add(vel, conditional(y, vel))))))), conditional(add(y, y), add(add(y, add(add(vel, x), add(x, x))), add(x, y))))</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-2124.17</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-2086.43</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-2219.44</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-2489.29</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-2528.56</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-2514.32</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-2445.12</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-2356.86</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-2171.2</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-2067.86</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-1834.06</v>
+      </c>
+      <c r="M6" t="n">
+        <v>-1925.51</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-1949.95</v>
+      </c>
+      <c r="O6" t="n">
+        <v>-1948.11</v>
+      </c>
+      <c r="P6" t="n">
+        <v>-1963.7</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-2116.6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>conditional(add(y, add(y, y)), add(add(add(x, add(add(add(conditional(conditional(x, add(conditional(x, x), conditional(conditional(add(vel, y), x), y))), conditional(x, y)), add(add(y, x), conditional(conditional(conditional(vel, conditional(y, conditional(y, y))), conditional(add(x, y), conditional(x, x))), conditional(add(vel, y), conditional(add(x, y), conditional(conditional(conditional(conditional(add(x, vel), add(conditional(x, x), conditional(x, x))), vel), conditional(vel, y)), vel)))))), x), vel)), add(add(x, y), add(x, y))), vel))</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>-1626.2</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-1429.15</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-1244.09</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-1171.91</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-1222.53</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-1337.19</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-1254.79</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-1049.36</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-1665.77</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-1762.01</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-1911.21</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-1935.97</v>
+      </c>
+      <c r="N7" t="n">
+        <v>-2021.68</v>
+      </c>
+      <c r="O7" t="n">
+        <v>-2079.35</v>
+      </c>
+      <c r="P7" t="n">
+        <v>-2116.13</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-2145.25</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>add(conditional(x, conditional(vel, add(conditional(conditional(conditional(y, x), conditional(conditional(conditional(conditional(y, x), conditional(conditional(conditional(add(x, y), vel), add(x, y)), add(x, add(conditional(conditional(vel, x), add(x, y)), conditional(y, vel))))), conditional(add(add(conditional(conditional(y, y), conditional(y, vel)), vel), y), y)), add(x, add(conditional(conditional(vel, x), add(x, y)), conditional(y, vel))))), conditional(add(add(conditional(conditional(y, y), conditional(y, vel)), vel), y), y)), add(add(add(x, add(x, conditional(conditional(vel, vel), add(add(y, add(add(y, x), conditional(x, vel))), vel)))), conditional(conditional(conditional(add(x, x), conditional(y, x)), y), conditional(conditional(x, conditional(y, conditional(add(vel, vel), add(conditional(add(y, x), add(y, y)), conditional(conditional(x, y), x))))), add(vel, add(add(conditional(vel, x), conditional(conditional(add(x, add(vel, x)), conditional(x, vel)), vel)), conditional(add(y, add(add(conditional(vel, conditional(conditional(x, y), conditional(y, vel))), add(vel, y)), add(y, add(conditional(add(y, y), y), conditional(y, vel))))), x)))))), x)))), conditional(add(y, y), add(add(add(add(x, add(x, y)), y), add(vel, conditional(x, x))), x)))</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-2156.57</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-2145.19</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-2101.42</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-2404.31</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-2371.79</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-2333.31</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-2239.19</v>
+      </c>
+      <c r="I8" t="n">
+        <v>-2136.95</v>
+      </c>
+      <c r="J8" t="n">
+        <v>-2105.3</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-2030.5</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-1901.77</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-1699.11</v>
+      </c>
+      <c r="N8" t="n">
+        <v>-1767.64</v>
+      </c>
+      <c r="O8" t="n">
+        <v>-1868.14</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-1848.14</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-2045.28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finish editing memory gravity results
</commit_message>
<xml_diff>
--- a/pendulum/full_obs_pendulum/full_obs_grav.xlsx
+++ b/pendulum/full_obs_pendulum/full_obs_grav.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="500" windowWidth="18200" windowHeight="8500" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="500" windowWidth="18200" windowHeight="8500" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="9.81" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="11" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="12" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="13" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -6271,4 +6272,573 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>add(add(conditional(conditional(conditional(x, conditional(conditional(conditional(add(conditional(x, vel), conditional(vel, y)), x), conditional(add(add(x, conditional(vel, y)), conditional(x, y)), conditional(y, y))), vel)), add(add(vel, conditional(add(y, conditional(y, vel)), add(add(conditional(x, vel), add(x, y)), conditional(add(add(add(y, vel), y), conditional(y, y)), add(y, add(add(conditional(conditional(y, y), conditional(vel, vel)), add(add(x, y), add(vel, conditional(conditional(y, y), add(y, y))))), x)))))), conditional(conditional(conditional(conditional(y, y), x), conditional(add(y, conditional(add(x, x), y)), conditional(add(vel, x), conditional(add(x, conditional(x, x)), x)))), add(conditional(add(x, y), x), add(add(x, y), x))))), add(vel, vel)), conditional(x, add(x, conditional(x, vel)))), conditional(add(add(y, y), conditional(y, y)), add(add(x, add(x, y)), add(add(x, add(add(y, vel), add(x, y))), x))))</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>-1944.09</v>
+      </c>
+      <c r="C1" t="n">
+        <v>-1983.23</v>
+      </c>
+      <c r="D1" t="n">
+        <v>-1833.96</v>
+      </c>
+      <c r="E1" t="n">
+        <v>-1818.42</v>
+      </c>
+      <c r="F1" t="n">
+        <v>-1901.66</v>
+      </c>
+      <c r="G1" t="n">
+        <v>-2186.24</v>
+      </c>
+      <c r="H1" t="n">
+        <v>-2240.38</v>
+      </c>
+      <c r="I1" t="n">
+        <v>-2185.09</v>
+      </c>
+      <c r="J1" t="n">
+        <v>-1957.49</v>
+      </c>
+      <c r="K1" t="n">
+        <v>-2034.13</v>
+      </c>
+      <c r="L1" t="n">
+        <v>-1954.08</v>
+      </c>
+      <c r="M1" t="n">
+        <v>-1882.37</v>
+      </c>
+      <c r="N1" t="n">
+        <v>-1695.86</v>
+      </c>
+      <c r="O1" t="n">
+        <v>-1783.76</v>
+      </c>
+      <c r="P1" t="n">
+        <v>-1827.98</v>
+      </c>
+      <c r="Q1" t="n">
+        <v>-2003.01</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>conditional(add(add(y, add(y, y)), conditional(x, conditional(add(add(vel, conditional(y, conditional(x, conditional(add(x, vel), conditional(x, x))))), add(add(add(vel, x), add(y, add(y, y))), vel)), add(add(vel, vel), conditional(x, y))))), add(add(add(add(x, add(add(x, x), y)), add(y, x)), y), add(vel, x)))</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-1532.59</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-1348.34</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-1454.23</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-1411.54</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-1712.81</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-2032.2</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-1951.16</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-1903.98</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-1652.67</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-1812.1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-1937.5</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-2096.37</v>
+      </c>
+      <c r="N2" t="n">
+        <v>-2144.27</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-2203.32</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-2265.96</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-2312.92</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>conditional(add(y, add(y, y)), add(add(add(add(vel, add(x, y)), conditional(x, conditional(add(x, vel), conditional(x, vel)))), add(add(x, add(x, x)), add(add(y, x), y))), conditional(x, add(conditional(y, add(x, add(add(add(conditional(vel, x), add(add(x, x), add(conditional(conditional(add(x, y), add(add(conditional(x, y), conditional(y, vel)), conditional(x, vel))), y), conditional(vel, y)))), add(x, add(add(add(x, x), add(add(x, y), x)), add(y, conditional(x, conditional(conditional(vel, add(conditional(vel, x), conditional(x, y))), conditional(vel, vel))))))), conditional(conditional(vel, y), x)))), x))))</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>-1367.22</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-1389.54</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-1204.39</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-1231.77</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-1499.2</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-1654.53</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-1507.57</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-1476.15</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-1589.78</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-1747.01</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-1898.52</v>
+      </c>
+      <c r="M3" t="n">
+        <v>-1984.07</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-2039.43</v>
+      </c>
+      <c r="O3" t="n">
+        <v>-2074.51</v>
+      </c>
+      <c r="P3" t="n">
+        <v>-2145.55</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-2185.22</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>conditional(add(conditional(y, y), add(add(y, y), x)), add(conditional(vel, add(conditional(add(conditional(add(vel, vel), add(add(x, add(conditional(vel, add(x, x)), add(add(conditional(y, add(x, add(add(vel, x), conditional(x, x)))), conditional(vel, x)), add(y, x)))), x)), x), conditional(add(conditional(x, vel), add(x, y)), y)), vel)), add(add(vel, x), add(add(x, vel), add(add(add(conditional(x, conditional(x, x)), add(add(y, x), add(x, x))), add(add(conditional(conditional(add(x, conditional(y, vel)), y), x), x), add(add(add(add(conditional(x, x), conditional(add(x, y), conditional(y, vel))), add(x, x)), add(x, vel)), vel))), add(conditional(x, vel), add(x, y)))))))</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-1405.15</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-1481.18</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-1363.35</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-1609.2</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-1718.3</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-1584.89</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-1701.55</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-1608.97</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-1320.43</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-1549.2</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-1644.83</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-1775.87</v>
+      </c>
+      <c r="N4" t="n">
+        <v>-1870.54</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-1975.6</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-2054.64</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-2111.4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>conditional(add(add(conditional(y, y), x), add(y, y)), add(add(add(add(add(add(x, x), add(add(add(vel, conditional(x, x)), add(x, add(x, x))), vel)), conditional(y, vel)), add(x, y)), add(vel, x)), add(x, add(conditional(add(add(add(y, x), add(x, x)), conditional(conditional(vel, x), add(x, add(x, x)))), y), add(conditional(y, vel), x)))))</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-1640.62</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-1632.89</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-1551.49</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-1626.25</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-1739.95</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-1574.58</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-1713.68</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-1658.51</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-1275.59</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-1500.89</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-1686.05</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-1774.19</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-1857.16</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-1974.98</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-2039.42</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-2123.3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>add(add(conditional(x, add(conditional(x, x), add(conditional(conditional(x, x), add(conditional(conditional(add(vel, y), conditional(x, x)), add(vel, conditional(y, add(add(y, vel), add(x, conditional(add(y, x), conditional(x, vel))))))), add(add(vel, vel), vel))), conditional(y, conditional(conditional(vel, y), add(y, y)))))), conditional(y, add(conditional(x, add(vel, x)), add(add(add(conditional(x, x), y), x), add(conditional(vel, vel), add(conditional(add(vel, y), add(vel, x)), x)))))), conditional(add(y, y), add(add(add(x, vel), x), add(add(y, add(y, add(x, x))), conditional(x, x)))))</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-2265.91</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-2277.55</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-2235.43</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-2255.4</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-2272.83</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-2266.74</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-2221.49</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-2134.59</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-2062.02</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-1664.44</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-1653.9</v>
+      </c>
+      <c r="M6" t="n">
+        <v>-1738.8</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-1834.98</v>
+      </c>
+      <c r="O6" t="n">
+        <v>-1858.45</v>
+      </c>
+      <c r="P6" t="n">
+        <v>-1917.04</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-2042.67</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>add(conditional(y, add(add(add(x, y), conditional(y, add(conditional(add(vel, y), add(conditional(x, y), conditional(vel, x))), conditional(conditional(add(add(add(add(y, x), vel), conditional(vel, conditional(add(x, y), vel))), add(add(conditional(conditional(y, vel), y), x), y)), x), conditional(conditional(x, x), add(conditional(add(add(conditional(y, vel), conditional(vel, conditional(conditional(conditional(conditional(y, x), conditional(y, y)), y), conditional(x, x)))), x), conditional(vel, vel)), conditional(y, conditional(y, conditional(vel, conditional(y, add(vel, conditional(conditional(add(x, x), add(x, y)), add(y, vel))))))))))))), add(y, x))), conditional(add(conditional(conditional(x, y), conditional(y, x)), vel), add(add(y, vel), y)))</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>-2200.93</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-1790.35</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-1943.59</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-2177.36</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-2425.9</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-2432.09</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-2394.43</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-2389.31</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-2260.74</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-2160.22</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-1992.69</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-1733.56</v>
+      </c>
+      <c r="N7" t="n">
+        <v>-1753.67</v>
+      </c>
+      <c r="O7" t="n">
+        <v>-1842.77</v>
+      </c>
+      <c r="P7" t="n">
+        <v>-1840.54</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-2014.42</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>conditional(add(add(add(y, y), add(y, y)), conditional(y, x)), add(add(x, x), add(vel, add(add(add(add(x, x), conditional(x, add(add(y, add(conditional(x, x), x)), add(add(vel, conditional(x, y)), conditional(conditional(x, y), conditional(add(conditional(conditional(vel, y), add(x, x)), add(y, y)), add(add(y, conditional(y, y)), add(vel, vel)))))))), conditional(y, conditional(conditional(y, y), conditional(x, y)))), add(conditional(conditional(x, vel), add(add(x, vel), add(vel, conditional(conditional(x, conditional(y, vel)), conditional(add(add(y, y), add(y, vel)), conditional(add(conditional(add(vel, vel), conditional(conditional(conditional(vel, y), add(x, vel)), y)), y), add(vel, vel))))))), add(x, add(x, add(add(y, vel), add(y, add(conditional(y, y), add(x, add(x, y))))))))))))</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-1300.48</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-1245.68</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-1176.57</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-1359.83</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-1500.25</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-1508.47</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-1525.02</v>
+      </c>
+      <c r="I8" t="n">
+        <v>-1161.59</v>
+      </c>
+      <c r="J8" t="n">
+        <v>-1792.99</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-1912.36</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-1947.28</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-2030.01</v>
+      </c>
+      <c r="N8" t="n">
+        <v>-2064.98</v>
+      </c>
+      <c r="O8" t="n">
+        <v>-2109.59</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-2162.34</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-2227.2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>conditional(add(add(conditional(x, vel), y), y), add(add(x, add(y, add(conditional(x, add(vel, y)), add(add(x, x), add(conditional(add(x, conditional(y, conditional(x, x))), add(conditional(conditional(conditional(y, y), add(add(x, conditional(y, conditional(y, x))), add(conditional(y, add(conditional(x, x), add(x, y))), add(x, vel)))), x), x)), x))))), add(x, vel)))</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-1969.85</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-2006.03</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-1960.89</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-1920.7</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-1844.64</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-1759.9</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-1630.09</v>
+      </c>
+      <c r="I9" t="n">
+        <v>-1543.47</v>
+      </c>
+      <c r="J9" t="n">
+        <v>-1227.27</v>
+      </c>
+      <c r="K9" t="n">
+        <v>-1575.49</v>
+      </c>
+      <c r="L9" t="n">
+        <v>-1722.7</v>
+      </c>
+      <c r="M9" t="n">
+        <v>-1869.59</v>
+      </c>
+      <c r="N9" t="n">
+        <v>-1928.89</v>
+      </c>
+      <c r="O9" t="n">
+        <v>-2041.11</v>
+      </c>
+      <c r="P9" t="n">
+        <v>-2082.8</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>-2137.56</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>add(conditional(add(y, y), add(vel, add(x, add(add(add(x, add(x, x)), add(x, y)), y)))), conditional(conditional(x, x), conditional(add(x, x), add(add(conditional(add(conditional(vel, vel), y), conditional(vel, y)), vel), add(add(x, x), add(add(conditional(y, conditional(add(add(add(add(y, y), conditional(y, y)), x), vel), conditional(y, conditional(x, vel)))), vel), y))))))</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-2468.96</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-2424.31</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-2469.91</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-2483.38</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-2469.63</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-2417.33</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-2343.88</v>
+      </c>
+      <c r="I10" t="n">
+        <v>-2251.9</v>
+      </c>
+      <c r="J10" t="n">
+        <v>-2015.02</v>
+      </c>
+      <c r="K10" t="n">
+        <v>-2124.34</v>
+      </c>
+      <c r="L10" t="n">
+        <v>-2045.81</v>
+      </c>
+      <c r="M10" t="n">
+        <v>-1618.21</v>
+      </c>
+      <c r="N10" t="n">
+        <v>-1725.54</v>
+      </c>
+      <c r="O10" t="n">
+        <v>-1777.62</v>
+      </c>
+      <c r="P10" t="n">
+        <v>-1801.76</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>-1989.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>